<commit_message>
Planilha de requisitos validada
</commit_message>
<xml_diff>
--- a/documentação/Requisitos/Planilha de Requisitos.xlsx
+++ b/documentação/Requisitos/Planilha de Requisitos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
   <si>
     <t>Banco de dados</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Emitir alertas via slack ou telegram</t>
   </si>
   <si>
-    <t>Gerar relatório.</t>
-  </si>
-  <si>
     <t>Emitir alertas diarios com base nos quartis.</t>
   </si>
   <si>
@@ -77,20 +74,50 @@
     <t>Status de condição da maquina para usuario e Técnico</t>
   </si>
   <si>
-    <t>Tela de login e cadastro</t>
-  </si>
-  <si>
     <t>Conexão do sistema com a nuvem (AWS ou AZURE)</t>
   </si>
   <si>
     <t>Sistema disponivel em multiplataforma</t>
+  </si>
+  <si>
+    <t>Diego</t>
+  </si>
+  <si>
+    <t>Maycon</t>
+  </si>
+  <si>
+    <t>Igor</t>
+  </si>
+  <si>
+    <t>Jorge</t>
+  </si>
+  <si>
+    <t>José</t>
+  </si>
+  <si>
+    <t>Escala de dificulade fibonacci 1, 2, 3, 5, 8, 13, 21</t>
+  </si>
+  <si>
+    <t>Tela de login e cadastro funcional</t>
+  </si>
+  <si>
+    <t>Gerar relatório com base em dados capturados.</t>
+  </si>
+  <si>
+    <t>média</t>
+  </si>
+  <si>
+    <t>Arredondamento</t>
+  </si>
+  <si>
+    <t>Somatoria dos pontos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,8 +139,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -132,8 +166,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -200,21 +246,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -252,21 +283,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -293,12 +309,21 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
@@ -306,14 +331,117 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -322,16 +450,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -339,29 +491,42 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -643,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:F16"/>
+  <dimension ref="D2:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -654,161 +819,482 @@
     <col min="4" max="4" width="89.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:6" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="4:6" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="4:16" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="4:16" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="4:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="3" t="s">
+      <c r="G3" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="4:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="E4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="4:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="6" t="s">
+      <c r="G4" s="21">
+        <v>13</v>
+      </c>
+      <c r="H4" s="22">
+        <v>5</v>
+      </c>
+      <c r="I4" s="22">
+        <v>13</v>
+      </c>
+      <c r="J4" s="22">
+        <v>5</v>
+      </c>
+      <c r="K4" s="22">
+        <v>13</v>
+      </c>
+      <c r="L4" s="25">
+        <f>AVERAGE(G4:K4)</f>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="M4" s="19">
+        <v>8</v>
+      </c>
+      <c r="P4">
+        <f>SUM(M4:M16)</f>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="4:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="8" t="s">
+      <c r="E5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="4:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="9" t="s">
+      <c r="G5" s="21">
+        <v>13</v>
+      </c>
+      <c r="H5" s="22">
+        <v>8</v>
+      </c>
+      <c r="I5" s="22">
+        <v>21</v>
+      </c>
+      <c r="J5" s="22">
+        <v>13</v>
+      </c>
+      <c r="K5" s="22">
+        <v>8</v>
+      </c>
+      <c r="L5" s="25">
+        <f t="shared" ref="L5:L16" si="0">AVERAGE(G5:K5)</f>
+        <v>12.6</v>
+      </c>
+      <c r="M5" s="19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="4:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="8" t="s">
+      <c r="E6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="4:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="7" t="s">
+      <c r="G6" s="21">
+        <v>8</v>
+      </c>
+      <c r="H6" s="22">
+        <v>5</v>
+      </c>
+      <c r="I6" s="22">
+        <v>8</v>
+      </c>
+      <c r="J6" s="22">
+        <v>13</v>
+      </c>
+      <c r="K6" s="22">
+        <v>8</v>
+      </c>
+      <c r="L6" s="25">
+        <f t="shared" si="0"/>
+        <v>8.4</v>
+      </c>
+      <c r="M6" s="19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="4:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="4:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="6" t="s">
+      <c r="G7" s="21">
+        <v>5</v>
+      </c>
+      <c r="H7" s="22">
+        <v>5</v>
+      </c>
+      <c r="I7" s="22">
+        <v>8</v>
+      </c>
+      <c r="J7" s="22">
+        <v>8</v>
+      </c>
+      <c r="K7" s="22">
+        <v>5</v>
+      </c>
+      <c r="L7" s="25">
+        <f t="shared" si="0"/>
+        <v>6.2</v>
+      </c>
+      <c r="M7" s="19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="4:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="21">
+        <v>5</v>
+      </c>
+      <c r="H8" s="22">
+        <v>5</v>
+      </c>
+      <c r="I8" s="22">
+        <v>13</v>
+      </c>
+      <c r="J8" s="22">
+        <v>13</v>
+      </c>
+      <c r="K8" s="22">
+        <v>13</v>
+      </c>
+      <c r="L8" s="25">
+        <f t="shared" si="0"/>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="M8" s="19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="4:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="21">
+        <v>13</v>
+      </c>
+      <c r="H9" s="22">
+        <v>3</v>
+      </c>
+      <c r="I9" s="22">
+        <v>8</v>
+      </c>
+      <c r="J9" s="22">
+        <v>13</v>
+      </c>
+      <c r="K9" s="22">
+        <v>13</v>
+      </c>
+      <c r="L9" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M9" s="19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="4:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="21">
+        <v>21</v>
+      </c>
+      <c r="H10" s="22">
+        <v>8</v>
+      </c>
+      <c r="I10" s="22">
+        <v>21</v>
+      </c>
+      <c r="J10" s="22">
+        <v>8</v>
+      </c>
+      <c r="K10" s="22">
+        <v>8</v>
+      </c>
+      <c r="L10" s="25">
+        <f t="shared" si="0"/>
+        <v>13.2</v>
+      </c>
+      <c r="M10" s="19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="4:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="21">
+        <v>21</v>
+      </c>
+      <c r="H11" s="22">
+        <v>5</v>
+      </c>
+      <c r="I11" s="22">
+        <v>8</v>
+      </c>
+      <c r="J11" s="22">
+        <v>5</v>
+      </c>
+      <c r="K11" s="22">
+        <v>21</v>
+      </c>
+      <c r="L11" s="25">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="8" t="s">
+      <c r="M11" s="19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="4:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="4:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="8" t="s">
+      <c r="G12" s="21">
+        <v>3</v>
+      </c>
+      <c r="H12" s="22">
+        <v>3</v>
+      </c>
+      <c r="I12" s="22">
+        <v>3</v>
+      </c>
+      <c r="J12" s="22">
+        <v>3</v>
+      </c>
+      <c r="K12" s="22">
+        <v>3</v>
+      </c>
+      <c r="L12" s="25">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="M12" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="4:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="4:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="8" t="s">
+      <c r="G13" s="21">
+        <v>13</v>
+      </c>
+      <c r="H13" s="22">
+        <v>5</v>
+      </c>
+      <c r="I13" s="22">
+        <v>5</v>
+      </c>
+      <c r="J13" s="22">
+        <v>8</v>
+      </c>
+      <c r="K13" s="22">
+        <v>5</v>
+      </c>
+      <c r="L13" s="25">
+        <f t="shared" si="0"/>
+        <v>7.2</v>
+      </c>
+      <c r="M13" s="19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="4:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="4:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="8" t="s">
+      <c r="G14" s="21">
+        <v>13</v>
+      </c>
+      <c r="H14" s="22">
+        <v>5</v>
+      </c>
+      <c r="I14" s="22">
+        <v>13</v>
+      </c>
+      <c r="J14" s="22">
+        <v>8</v>
+      </c>
+      <c r="K14" s="22">
+        <v>8</v>
+      </c>
+      <c r="L14" s="25">
+        <f t="shared" si="0"/>
+        <v>9.4</v>
+      </c>
+      <c r="M14" s="19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="4:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="4:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="8" t="s">
+      <c r="G15" s="21">
+        <v>5</v>
+      </c>
+      <c r="H15" s="22">
+        <v>5</v>
+      </c>
+      <c r="I15" s="22">
+        <v>5</v>
+      </c>
+      <c r="J15" s="22">
+        <v>5</v>
+      </c>
+      <c r="K15" s="22">
+        <v>5</v>
+      </c>
+      <c r="L15" s="25">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="M15" s="19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="4:16" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="4:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="4:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="4:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="4:6" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>6</v>
+      <c r="G16" s="23">
+        <v>13</v>
+      </c>
+      <c r="H16" s="24">
+        <v>3</v>
+      </c>
+      <c r="I16" s="24">
+        <v>5</v>
+      </c>
+      <c r="J16" s="24">
+        <v>3</v>
+      </c>
+      <c r="K16" s="24">
+        <v>3</v>
+      </c>
+      <c r="L16" s="26">
+        <f t="shared" si="0"/>
+        <v>5.4</v>
+      </c>
+      <c r="M16" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="15" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
User Stories | Correção de arquivos
</commit_message>
<xml_diff>
--- a/documentação/Requisitos/Planilha de Requisitos.xlsx
+++ b/documentação/Requisitos/Planilha de Requisitos.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cliente\Desktop\Fastech\documentação\Requisitos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josel\OneDrive\Área de Trabalho\work\Fastech\documentação\Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A912F490-3C41-4C1A-8687-8DE27634C0D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha de requisitos" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -116,7 +125,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -450,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -527,6 +536,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -807,20 +819,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D2:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="89.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="4:16" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -891,7 +904,7 @@
       <c r="M4" s="19">
         <v>8</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="27">
         <f>SUM(M4:M16)</f>
         <v>105</v>
       </c>

</xml_diff>

<commit_message>
RFT 2 D Modificacao do requisitos
</commit_message>
<xml_diff>
--- a/documentação/Requisitos/Planilha de Requisitos.xlsx
+++ b/documentação/Requisitos/Planilha de Requisitos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josel\OneDrive\Área de Trabalho\work\Fastech\documentação\Requisitos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igorf\Documents\Fastech\documentação\Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A912F490-3C41-4C1A-8687-8DE27634C0D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC71B9E7-D912-482B-B0F5-A87D16E4F0E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t>Banco de dados</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>Somatoria dos pontos</t>
+  </si>
+  <si>
+    <t>Não Funcional</t>
   </si>
 </sst>
 </file>
@@ -459,7 +462,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -540,6 +543,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -823,7 +827,7 @@
   <dimension ref="D2:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -836,7 +840,9 @@
     <col min="16" max="16" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:16" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="4:16" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="28"/>
+    </row>
     <row r="3" spans="4:16" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" s="1" t="s">
         <v>2</v>
@@ -1214,7 +1220,7 @@
         <v>5</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="G14" s="21">
         <v>13</v>
@@ -1247,7 +1253,7 @@
         <v>8</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="G15" s="21">
         <v>5</v>
@@ -1312,6 +1318,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>